<commit_message>
New tool added & goodbye message
</commit_message>
<xml_diff>
--- a/orarFiles/Orar.xlsx
+++ b/orarFiles/Orar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{780A9EE5-49B5-4304-8364-5DC31E219F1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5E4A508-0367-4335-A6D0-60FDA031BD07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Ziua</t>
   </si>
@@ -28,6 +28,12 @@
     <t>Ora</t>
   </si>
   <si>
+    <t>8 → 9</t>
+  </si>
+  <si>
+    <t>9 → 10</t>
+  </si>
+  <si>
     <t>10 → 11</t>
   </si>
   <si>
@@ -56,160 +62,16 @@
   </si>
   <si>
     <t>Vineri</t>
-  </si>
-  <si>
-    <t>Mate</t>
-  </si>
-  <si>
-    <t>Geogra</t>
-  </si>
-  <si>
-    <t>Sport</t>
-  </si>
-  <si>
-    <t>Biologie</t>
-  </si>
-  <si>
-    <t>15 → 16</t>
-  </si>
-  <si>
-    <t>16 → 17</t>
-  </si>
-  <si>
-    <t>17 → 18</t>
-  </si>
-  <si>
-    <t>18 → 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - </t>
-  </si>
-  <si>
-    <t>Română</t>
-  </si>
-  <si>
-    <t>Engleză</t>
-  </si>
-  <si>
-    <t>Fizică</t>
-  </si>
-  <si>
-    <t>Germană</t>
-  </si>
-  <si>
-    <t>Filozofie</t>
-  </si>
-  <si>
-    <t>Rom. Opt.</t>
-  </si>
-  <si>
-    <t>Rom. Extr.</t>
-  </si>
-  <si>
-    <t>Dirigenție</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Portocaliu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Ore extra, nu fac parte din orarul oficial</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Gri</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Doar pentru cei cu BAC sau pentru cei la care se aplică</t>
-    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -242,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -357,20 +219,11 @@
         <color auto="1"/>
       </diagonal>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -402,20 +255,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="256" zoomScaleNormal="256" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,19 +616,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -808,218 +647,80 @@
         <v>2</v>
       </c>
       <c r="B3" s="10"/>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="10"/>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A13:G13"/>
+  <mergeCells count="12">
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A3:B3"/>
@@ -1033,7 +734,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>